<commit_message>
push pending all for long time
</commit_message>
<xml_diff>
--- a/src/Documents/Day_log_work.xlsx
+++ b/src/Documents/Day_log_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Practice\src\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15510E6-7EDB-41E2-A79B-700B5F3DE997}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7BFA80-0B9F-4D39-BB76-C480DB692DBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="827">
   <si>
     <t>Ticket_id</t>
   </si>
@@ -2505,6 +2505,24 @@
   </si>
   <si>
     <t>kibana visuatigation fail in CI</t>
+  </si>
+  <si>
+    <t>support for 3uk</t>
+  </si>
+  <si>
+    <t>node not ready</t>
+  </si>
+  <si>
+    <t>spring training</t>
+  </si>
+  <si>
+    <t>spring training + 5g csd</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>csd</t>
   </si>
 </sst>
 </file>
@@ -11919,8 +11937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA16314-1EBD-45FC-BE59-12C57F1884F2}">
   <dimension ref="A1:R366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="C305" sqref="C305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11942,7 +11960,7 @@
     <col min="18" max="18" width="38.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="174" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -12044,7 +12062,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3817</v>
       </c>
@@ -12073,7 +12091,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3817</v>
       </c>
@@ -12183,7 +12201,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3835</v>
       </c>
@@ -12276,7 +12294,7 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
     </row>
-    <row r="12" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3835</v>
       </c>
@@ -12410,7 +12428,7 @@
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
     </row>
-    <row r="18" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="174" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3835</v>
       </c>
@@ -12525,7 +12543,7 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
     </row>
-    <row r="22" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3835</v>
       </c>
@@ -12652,7 +12670,7 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
     </row>
-    <row r="26" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>617</v>
       </c>
@@ -12713,7 +12731,7 @@
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="174" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>4269</v>
       </c>
@@ -12749,7 +12767,7 @@
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
     </row>
-    <row r="30" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="145" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4269</v>
       </c>
@@ -12823,7 +12841,7 @@
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>4282</v>
       </c>
@@ -12855,7 +12873,7 @@
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
     </row>
-    <row r="33" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>633</v>
       </c>
@@ -12935,7 +12953,7 @@
       </c>
       <c r="O35" s="13"/>
     </row>
-    <row r="36" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="232" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4282</v>
       </c>
@@ -13003,7 +13021,7 @@
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
     </row>
-    <row r="38" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>4227</v>
       </c>
@@ -13035,7 +13053,7 @@
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
     </row>
-    <row r="39" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>4287</v>
       </c>
@@ -13146,7 +13164,7 @@
       </c>
       <c r="O42" s="13"/>
     </row>
-    <row r="43" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>4287</v>
       </c>
@@ -13742,7 +13760,7 @@
       <c r="N67" s="13"/>
       <c r="O67" s="13"/>
     </row>
-    <row r="68" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="D68" s="12">
         <v>43532</v>
       </c>
@@ -13851,7 +13869,7 @@
       <c r="N72" s="13"/>
       <c r="O72" s="13"/>
     </row>
-    <row r="73" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>625</v>
       </c>
@@ -13948,7 +13966,7 @@
       <c r="N77" s="13"/>
       <c r="O77" s="13"/>
     </row>
-    <row r="78" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>4167</v>
       </c>
@@ -13980,7 +13998,7 @@
       <c r="N78" s="13"/>
       <c r="O78" s="13"/>
     </row>
-    <row r="79" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>4167</v>
       </c>
@@ -14012,7 +14030,7 @@
       <c r="N79" s="13"/>
       <c r="O79" s="13"/>
     </row>
-    <row r="80" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>4167</v>
       </c>
@@ -14044,7 +14062,7 @@
       <c r="N80" s="13"/>
       <c r="O80" s="13"/>
     </row>
-    <row r="81" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>4167</v>
       </c>
@@ -14076,7 +14094,7 @@
       <c r="N81" s="13"/>
       <c r="O81" s="13"/>
     </row>
-    <row r="82" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>4167</v>
       </c>
@@ -14142,7 +14160,7 @@
       <c r="N84" s="13"/>
       <c r="O84" s="13"/>
     </row>
-    <row r="85" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>625</v>
       </c>
@@ -15642,7 +15660,7 @@
       <c r="N162" s="12"/>
       <c r="O162" s="12"/>
     </row>
-    <row r="163" spans="2:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:15" ht="58" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>611</v>
       </c>
@@ -15666,7 +15684,7 @@
       <c r="N163" s="12"/>
       <c r="O163" s="12"/>
     </row>
-    <row r="164" spans="2:15" ht="116" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>611</v>
       </c>
@@ -15690,7 +15708,7 @@
       <c r="N164" s="12"/>
       <c r="O164" s="12"/>
     </row>
-    <row r="165" spans="2:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:15" ht="29" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>611</v>
       </c>
@@ -15714,7 +15732,7 @@
       <c r="N165" s="12"/>
       <c r="O165" s="12"/>
     </row>
-    <row r="166" spans="2:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:15" ht="58" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>625</v>
       </c>
@@ -15840,7 +15858,7 @@
       <c r="N172" s="12"/>
       <c r="O172" s="12"/>
     </row>
-    <row r="173" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D173" s="12">
         <v>43637</v>
       </c>
@@ -15891,7 +15909,7 @@
       <c r="N175" s="12"/>
       <c r="O175" s="12"/>
     </row>
-    <row r="176" spans="2:15" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="D176" s="12">
         <v>43640</v>
       </c>
@@ -15912,7 +15930,7 @@
       <c r="N176" s="12"/>
       <c r="O176" s="12"/>
     </row>
-    <row r="177" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="D177" s="12">
         <v>43641</v>
       </c>
@@ -15975,7 +15993,7 @@
       <c r="N179" s="12"/>
       <c r="O179" s="12"/>
     </row>
-    <row r="180" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D180" s="12">
         <v>43644</v>
       </c>
@@ -16056,7 +16074,7 @@
       <c r="N183" s="12"/>
       <c r="O183" s="12"/>
     </row>
-    <row r="184" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>4398</v>
       </c>
@@ -18312,10 +18330,18 @@
       <c r="O291" s="12"/>
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B292" t="s">
+        <v>611</v>
+      </c>
+      <c r="C292">
+        <v>8</v>
+      </c>
       <c r="D292" s="12">
         <v>43756</v>
       </c>
-      <c r="E292"/>
+      <c r="E292" t="s">
+        <v>81</v>
+      </c>
       <c r="I292" s="3"/>
       <c r="J292" s="3"/>
       <c r="K292" s="12"/>
@@ -18328,7 +18354,9 @@
       <c r="D293" s="12">
         <v>43757</v>
       </c>
-      <c r="E293"/>
+      <c r="E293" t="s">
+        <v>150</v>
+      </c>
       <c r="I293" s="3"/>
       <c r="J293" s="3"/>
       <c r="K293" s="12"/>
@@ -18341,7 +18369,9 @@
       <c r="D294" s="12">
         <v>43758</v>
       </c>
-      <c r="E294"/>
+      <c r="E294" t="s">
+        <v>150</v>
+      </c>
       <c r="I294" s="3"/>
       <c r="J294" s="3"/>
       <c r="K294" s="12"/>
@@ -18380,7 +18410,12 @@
       <c r="D297" s="12">
         <v>43761</v>
       </c>
-      <c r="E297"/>
+      <c r="E297" t="s">
+        <v>821</v>
+      </c>
+      <c r="F297" s="3" t="s">
+        <v>822</v>
+      </c>
       <c r="I297" s="3"/>
       <c r="J297" s="3"/>
       <c r="K297" s="12"/>
@@ -18393,7 +18428,9 @@
       <c r="D298" s="12">
         <v>43762</v>
       </c>
-      <c r="E298"/>
+      <c r="E298" t="s">
+        <v>821</v>
+      </c>
       <c r="I298" s="3"/>
       <c r="J298" s="3"/>
       <c r="K298" s="12"/>
@@ -18419,7 +18456,9 @@
       <c r="D300" s="12">
         <v>43764</v>
       </c>
-      <c r="E300"/>
+      <c r="E300" t="s">
+        <v>150</v>
+      </c>
       <c r="I300" s="3"/>
       <c r="J300" s="3"/>
       <c r="K300" s="12"/>
@@ -18432,7 +18471,9 @@
       <c r="D301" s="12">
         <v>43765</v>
       </c>
-      <c r="E301"/>
+      <c r="E301" t="s">
+        <v>150</v>
+      </c>
       <c r="I301" s="3"/>
       <c r="J301" s="3"/>
       <c r="K301" s="12"/>
@@ -18445,7 +18486,9 @@
       <c r="D302" s="12">
         <v>43766</v>
       </c>
-      <c r="E302"/>
+      <c r="E302" t="s">
+        <v>823</v>
+      </c>
       <c r="I302" s="3"/>
       <c r="J302" s="3"/>
       <c r="K302" s="12"/>
@@ -18458,7 +18501,9 @@
       <c r="D303" s="12">
         <v>43767</v>
       </c>
-      <c r="E303"/>
+      <c r="E303" t="s">
+        <v>823</v>
+      </c>
       <c r="I303" s="3"/>
       <c r="J303" s="3"/>
       <c r="K303" s="12"/>
@@ -18471,7 +18516,9 @@
       <c r="D304" s="12">
         <v>43768</v>
       </c>
-      <c r="E304"/>
+      <c r="E304" t="s">
+        <v>824</v>
+      </c>
       <c r="I304" s="3"/>
       <c r="J304" s="3"/>
       <c r="K304" s="12"/>
@@ -18481,10 +18528,18 @@
       <c r="O304" s="12"/>
     </row>
     <row r="305" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B305" t="s">
+        <v>625</v>
+      </c>
+      <c r="C305">
+        <v>8</v>
+      </c>
       <c r="D305" s="12">
         <v>43769</v>
       </c>
-      <c r="E305"/>
+      <c r="E305" t="s">
+        <v>81</v>
+      </c>
       <c r="I305" s="3"/>
       <c r="J305" s="3"/>
       <c r="K305" s="12"/>
@@ -18515,7 +18570,9 @@
       <c r="D307" s="12">
         <v>43771</v>
       </c>
-      <c r="E307"/>
+      <c r="E307" t="s">
+        <v>150</v>
+      </c>
       <c r="I307" s="3"/>
       <c r="J307" s="3"/>
       <c r="K307" s="12"/>
@@ -18528,7 +18585,9 @@
       <c r="D308" s="12">
         <v>43772</v>
       </c>
-      <c r="E308"/>
+      <c r="E308" t="s">
+        <v>150</v>
+      </c>
       <c r="I308" s="3"/>
       <c r="J308" s="3"/>
       <c r="K308" s="12"/>
@@ -18541,7 +18600,12 @@
       <c r="D309" s="12">
         <v>43773</v>
       </c>
-      <c r="E309"/>
+      <c r="E309" t="s">
+        <v>825</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>826</v>
+      </c>
       <c r="I309" s="3"/>
       <c r="J309" s="3"/>
       <c r="K309" s="12"/>

</xml_diff>